<commit_message>
made a copy of the ALUM 2020 data (currently locked) and altered workflow file to point to this new file
</commit_message>
<xml_diff>
--- a/NeapWorkflow_AllDatasetsForGeneratingOverlayGrids.xlsx
+++ b/NeapWorkflow_AllDatasetsForGeneratingOverlayGrids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/new298_csiro_au/Documents/Code/Python/NEAP/ecosystem-typology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="222" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B3B4FC3-2B95-47F2-B8A8-C66440DBA3D4}"/>
+  <xr:revisionPtr revIDLastSave="223" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13320FFE-0376-4DD9-92AB-E061BEFD144B}"/>
   <bookViews>
-    <workbookView xWindow="372" yWindow="360" windowWidth="24360" windowHeight="13752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8376" yWindow="828" windowWidth="28092" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -195,9 +195,6 @@
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\Lakes_NEAP_20240723.shp</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2020_21_prerelease2_20240724\ABARES_Land_use_of_Australia_2020_21_prerelease2_20240724\NLUM_v7p2_ALUMV8_250m_2020_21_alb.tif</t>
-  </si>
-  <si>
     <t>As above</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>Terrestrial-Extant-IUCNGET</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2020_21_prerelease2_20240724\ABARES_Land_use_of_Australia_2020_21_prerelease2_20240724\copy\NLUM_v7p2_ALUMV8_250m_2020_21_alb.tif</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -692,7 +692,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>42</v>
@@ -716,7 +716,7 @@
         <v>19</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
@@ -727,10 +727,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
@@ -751,7 +751,7 @@
         <v>19</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J5" t="s">
         <v>10</v>
@@ -894,15 +894,15 @@
         <v>16</v>
       </c>
       <c r="K9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>53</v>
       </c>
-      <c r="B10" t="s">
-        <v>56</v>
+      <c r="B10" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
@@ -929,7 +929,7 @@
         <v>16</v>
       </c>
       <c r="K10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -947,8 +947,9 @@
     <hyperlink ref="B6" r:id="rId11" xr:uid="{6D271174-0A26-4C2B-8A49-23E0D84CB50C}"/>
     <hyperlink ref="I5" r:id="rId12" xr:uid="{16F34F99-BF30-4669-8EFB-A623D8834027}"/>
     <hyperlink ref="B5" r:id="rId13" xr:uid="{738F1511-B6CE-4E2B-B259-2280CFB5917B}"/>
+    <hyperlink ref="B10" r:id="rId14" xr:uid="{6F04B0FF-A351-4BA7-A8CB-FFA1BA3FA44A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated path to Pre-1750 NVIS input data in the workflows
</commit_message>
<xml_diff>
--- a/NeapWorkflow_AllDatasetsForGeneratingOverlayGrids.xlsx
+++ b/NeapWorkflow_AllDatasetsForGeneratingOverlayGrids.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/new298_csiro_au/Documents/Code/Python/NEAP/ecosystem-typology/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\new298\OneDrive - CSIRO\Code\Python\NEAP\ecosystem-typology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="226" documentId="11_F25DC773A252ABDACC1048D7191B70705ADE5906" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{779ED673-CA79-44E4-929C-0C0B037D81AF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E2935D-C8A2-428C-8261-D7DC3B7344D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="696" windowWidth="28908" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20610" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -153,9 +153,6 @@
     <t>//fs1-cbr.nexus.csiro.au/{ev-neap}/work/extent/inputs/raw/Marine/NVE-Benthic/NESP-MERI_Natural_Values_Ecosystems_withVAT.tif</t>
   </si>
   <si>
-    <t>//fs1-cbr.nexus.csiro.au/{ev-neap}/work/extent/processing/NEAP_intermediate/NVIS_PRE1750_IUCNGET_DK_20240714.tif</t>
-  </si>
-  <si>
     <t>subject_label</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2020_21_prerelease2_20240724\NLUM_v7p2_ALUMV8_250m_2020_21_alb.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\NVIS_PRE1750_IUCNGET_DK_20240730.tif</t>
   </si>
 </sst>
 </file>
@@ -272,7 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -282,7 +282,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -567,25 +566,25 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="223" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="105.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="112.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.44140625" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="105.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="112.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -620,7 +619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -655,7 +654,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -663,7 +662,7 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
@@ -681,7 +680,7 @@
         <v>19</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J3" t="s">
         <v>5</v>
@@ -690,12 +689,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>42</v>
+        <v>59</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
@@ -716,7 +715,7 @@
         <v>19</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
@@ -725,12 +724,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
@@ -751,18 +750,18 @@
         <v>19</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
         <v>36</v>
@@ -783,16 +782,16 @@
         <v>26</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -818,7 +817,7 @@
         <v>26</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J7" t="s">
         <v>14</v>
@@ -827,9 +826,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
@@ -853,7 +852,7 @@
         <v>19</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J8" t="s">
         <v>16</v>
@@ -862,9 +861,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
         <v>23</v>
@@ -888,21 +887,21 @@
         <v>19</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J9" t="s">
         <v>16</v>
       </c>
       <c r="K9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
@@ -923,13 +922,13 @@
         <v>19</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J10" t="s">
         <v>16</v>
       </c>
       <c r="K10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -948,8 +947,9 @@
     <hyperlink ref="I5" r:id="rId12" xr:uid="{16F34F99-BF30-4669-8EFB-A623D8834027}"/>
     <hyperlink ref="B5" r:id="rId13" xr:uid="{738F1511-B6CE-4E2B-B259-2280CFB5917B}"/>
     <hyperlink ref="B10" r:id="rId14" xr:uid="{6F04B0FF-A351-4BA7-A8CB-FFA1BA3FA44A}"/>
+    <hyperlink ref="B4" r:id="rId15" xr:uid="{798E46A6-7D89-4A9E-A128-06DE5D2BF74E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated all workflow files with new path to NVIS Extant and Pre1750 files
</commit_message>
<xml_diff>
--- a/NeapWorkflow_AllDatasetsForGeneratingOverlayGrids.xlsx
+++ b/NeapWorkflow_AllDatasetsForGeneratingOverlayGrids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\new298\OneDrive - CSIRO\Code\Python\NEAP\ecosystem-typology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E2935D-C8A2-428C-8261-D7DC3B7344D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C14E3BC-42DC-47EC-91EB-27434DC5A4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20610" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16515" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -195,9 +195,6 @@
     <t>As above</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\NVIS_IUCNGET_DK_20240709.tif</t>
-  </si>
-  <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\overlay_grids\Terrestrial_Pre1750_EPSG3577_250m.tif</t>
   </si>
   <si>
@@ -213,7 +210,10 @@
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2020_21_prerelease2_20240724\NLUM_v7p2_ALUMV8_250m_2020_21_alb.tif</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\NVIS_PRE1750_IUCNGET_DK_20240730.tif</t>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\NVIS_PRE1750_IUCNGET_DK_20240801.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\NVIS_IUCNGET_DK_20240801.tif</t>
   </si>
 </sst>
 </file>
@@ -565,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,10 +691,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
@@ -715,7 +715,7 @@
         <v>19</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
@@ -726,10 +726,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
@@ -750,7 +750,7 @@
         <v>19</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J5" t="s">
         <v>10</v>
@@ -901,7 +901,7 @@
         <v>52</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Crosswalk NVIS FM1.3 to FM1.2 and revise the Lakes to no-overlap with ALUM reservoirs
</commit_message>
<xml_diff>
--- a/NeapWorkflow_AllDatasetsForGeneratingOverlayGrids.xlsx
+++ b/NeapWorkflow_AllDatasetsForGeneratingOverlayGrids.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\new298\OneDrive - CSIRO\Code\Python\NEAP\ecosystem-typology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu240\Downloads\ext\ecosystem-typology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C14E3BC-42DC-47EC-91EB-27434DC5A4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E18054-32F3-446E-A9BC-D27221C0BC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16515" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="20580" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -189,9 +189,6 @@
     <t>https://github.com/CSIRO-enviro-informatics/ecosystem-typology/raw/main/crosswalks/Geofabric-IUCNGET/Lacustrine-IUCNGET.xlsx</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\Lakes_NEAP_20240723.shp</t>
-  </si>
-  <si>
     <t>As above</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\NVIS_IUCNGET_DK_20240801.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\Lakes_NEAP_20240808_NoOverlapWithALUM.shp</t>
   </si>
 </sst>
 </file>
@@ -566,25 +566,25 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="223" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="105.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="112.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="105.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="112.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -619,7 +619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -654,7 +654,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -689,12 +689,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
@@ -715,7 +715,7 @@
         <v>19</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
@@ -724,12 +724,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
@@ -750,18 +750,18 @@
         <v>19</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>50</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>36</v>
@@ -791,7 +791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -826,7 +826,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -861,7 +861,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -893,15 +893,15 @@
         <v>16</v>
       </c>
       <c r="K9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
@@ -928,7 +928,7 @@
         <v>16</v>
       </c>
       <c r="K10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -943,13 +943,12 @@
     <hyperlink ref="I10" r:id="rId8" xr:uid="{8B471BD3-FA1D-4955-B103-79825EEF4FCB}"/>
     <hyperlink ref="B2" r:id="rId9" xr:uid="{4AAD34BE-AFA6-4C42-98A5-31EBD33DB2C2}"/>
     <hyperlink ref="J6" r:id="rId10" xr:uid="{9D2ED58A-1BCA-4AFA-A7DB-AC11216EF831}"/>
-    <hyperlink ref="B6" r:id="rId11" xr:uid="{6D271174-0A26-4C2B-8A49-23E0D84CB50C}"/>
-    <hyperlink ref="I5" r:id="rId12" xr:uid="{16F34F99-BF30-4669-8EFB-A623D8834027}"/>
-    <hyperlink ref="B5" r:id="rId13" xr:uid="{738F1511-B6CE-4E2B-B259-2280CFB5917B}"/>
-    <hyperlink ref="B10" r:id="rId14" xr:uid="{6F04B0FF-A351-4BA7-A8CB-FFA1BA3FA44A}"/>
-    <hyperlink ref="B4" r:id="rId15" xr:uid="{798E46A6-7D89-4A9E-A128-06DE5D2BF74E}"/>
+    <hyperlink ref="I5" r:id="rId11" xr:uid="{16F34F99-BF30-4669-8EFB-A623D8834027}"/>
+    <hyperlink ref="B5" r:id="rId12" xr:uid="{738F1511-B6CE-4E2B-B259-2280CFB5917B}"/>
+    <hyperlink ref="B10" r:id="rId13" xr:uid="{6F04B0FF-A351-4BA7-A8CB-FFA1BA3FA44A}"/>
+    <hyperlink ref="B4" r:id="rId14" xr:uid="{798E46A6-7D89-4A9E-A128-06DE5D2BF74E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update the latest full NLUM data path
</commit_message>
<xml_diff>
--- a/NeapWorkflow_AllDatasetsForGeneratingOverlayGrids.xlsx
+++ b/NeapWorkflow_AllDatasetsForGeneratingOverlayGrids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu240\Downloads\ext\ecosystem-typology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E18054-32F3-446E-A9BC-D27221C0BC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBC9588-65EE-4A6A-9CED-EDCAC13526D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="20580" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -93,12 +93,6 @@
     <t>epsg:4283</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\NLUM_ALUMV8_250m_2010_11_alb\NLUM_ALUMV8_250m_2010_11_alb.tif</t>
-  </si>
-  <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\NLUM_ALUMV8_250m_2015_16_alb\NLUM_ALUMV8_250m_2015_16_alb.tif</t>
-  </si>
-  <si>
     <t>NN</t>
   </si>
   <si>
@@ -204,9 +198,6 @@
     <t>Terrestrial-Extant-IUCNGET</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2020_21_prerelease2_20240724\NLUM_v7p2_ALUMV8_250m_2020_21_alb.tif</t>
-  </si>
-  <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\NVIS_PRE1750_IUCNGET_DK_20240801.tif</t>
   </si>
   <si>
@@ -214,6 +205,15 @@
   </si>
   <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\Lakes_NEAP_20240808_NoOverlapWithALUM.shp</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2010_11_to_2020_21_prerelease3_20240809\NLUM_v7p3_ALUMV8_250m_2010_11_alb\NLUM_v7p3_ALUMV8_250m_2010_11_alb.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2010_11_to_2020_21_prerelease3_20240809\NLUM_v7p3_ALUMV8_250m_2015_16_alb\NLUM_v7p3_ALUMV8_250m_2015_16_alb.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2010_11_to_2020_21_prerelease3_20240809\NLUM_v7p3_ALUMV8_250m_2020_21_alb\NLUM_v7p3_ALUMV8_250m_2020_21_alb.tif</t>
   </si>
 </sst>
 </file>
@@ -566,36 +566,36 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="223" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.08984375" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="105.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="112.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.44140625" customWidth="1"/>
+    <col min="7" max="7" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="105.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="112.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -604,13 +604,13 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>0</v>
@@ -619,18 +619,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -645,7 +645,7 @@
         <v>19</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
@@ -654,18 +654,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -680,7 +680,7 @@
         <v>19</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J3" t="s">
         <v>5</v>
@@ -689,18 +689,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -715,7 +715,7 @@
         <v>19</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
@@ -724,18 +724,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -750,24 +750,24 @@
         <v>19</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -779,19 +779,19 @@
         <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -799,10 +799,10 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
         <v>20</v>
@@ -814,10 +814,10 @@
         <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J7" t="s">
         <v>14</v>
@@ -826,18 +826,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -846,13 +846,13 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H8" t="s">
         <v>19</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J8" t="s">
         <v>16</v>
@@ -861,18 +861,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -881,33 +881,33 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H9" t="s">
         <v>19</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J9" t="s">
         <v>16</v>
       </c>
       <c r="K9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -916,19 +916,19 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H10" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J10" t="s">
         <v>16</v>
       </c>
       <c r="K10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -945,10 +945,9 @@
     <hyperlink ref="J6" r:id="rId10" xr:uid="{9D2ED58A-1BCA-4AFA-A7DB-AC11216EF831}"/>
     <hyperlink ref="I5" r:id="rId11" xr:uid="{16F34F99-BF30-4669-8EFB-A623D8834027}"/>
     <hyperlink ref="B5" r:id="rId12" xr:uid="{738F1511-B6CE-4E2B-B259-2280CFB5917B}"/>
-    <hyperlink ref="B10" r:id="rId13" xr:uid="{6F04B0FF-A351-4BA7-A8CB-FFA1BA3FA44A}"/>
-    <hyperlink ref="B4" r:id="rId14" xr:uid="{798E46A6-7D89-4A9E-A128-06DE5D2BF74E}"/>
+    <hyperlink ref="B4" r:id="rId13" xr:uid="{798E46A6-7D89-4A9E-A128-06DE5D2BF74E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update to use lake only data
</commit_message>
<xml_diff>
--- a/NeapWorkflow_AllDatasetsForGeneratingOverlayGrids.xlsx
+++ b/NeapWorkflow_AllDatasetsForGeneratingOverlayGrids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu240\Downloads\ext\ecosystem-typology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBC9588-65EE-4A6A-9CED-EDCAC13526D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A097325-9C5A-40CE-B3CF-07030341A4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -204,9 +204,6 @@
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\NVIS_IUCNGET_DK_20240801.tif</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\Lakes_NEAP_20240808_NoOverlapWithALUM.shp</t>
-  </si>
-  <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2010_11_to_2020_21_prerelease3_20240809\NLUM_v7p3_ALUMV8_250m_2010_11_alb\NLUM_v7p3_ALUMV8_250m_2010_11_alb.tif</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\inputs\raw\Land_use_of_Australia\ABARES_Land_use_of_Australia_2010_11_to_2020_21_prerelease3_20240809\NLUM_v7p3_ALUMV8_250m_2020_21_alb\NLUM_v7p3_ALUMV8_250m_2020_21_alb.tif</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\Lakes_NEAP_20240723.shp</t>
   </si>
 </sst>
 </file>
@@ -566,7 +566,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -761,7 +761,7 @@
         <v>48</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
@@ -831,7 +831,7 @@
         <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
@@ -866,7 +866,7 @@
         <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
         <v>36</v>
@@ -901,7 +901,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
         <v>36</v>
@@ -946,8 +946,9 @@
     <hyperlink ref="I5" r:id="rId11" xr:uid="{16F34F99-BF30-4669-8EFB-A623D8834027}"/>
     <hyperlink ref="B5" r:id="rId12" xr:uid="{738F1511-B6CE-4E2B-B259-2280CFB5917B}"/>
     <hyperlink ref="B4" r:id="rId13" xr:uid="{798E46A6-7D89-4A9E-A128-06DE5D2BF74E}"/>
+    <hyperlink ref="B6" r:id="rId14" xr:uid="{F3A55584-386C-449A-B9B5-0BC12AC3DCF9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update NVIS pre derived data
</commit_message>
<xml_diff>
--- a/NeapWorkflow_AllDatasetsForGeneratingOverlayGrids.xlsx
+++ b/NeapWorkflow_AllDatasetsForGeneratingOverlayGrids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu240\Downloads\ext\ecosystem-typology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A097325-9C5A-40CE-B3CF-07030341A4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8CA82B-43BB-4E4A-AD17-8810298EC3F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -198,9 +198,6 @@
     <t>Terrestrial-Extant-IUCNGET</t>
   </si>
   <si>
-    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\NVIS_PRE1750_IUCNGET_DK_20240801.tif</t>
-  </si>
-  <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\NVIS_IUCNGET_DK_20240801.tif</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\Lakes_NEAP_20240723.shp</t>
+  </si>
+  <si>
+    <t>\\fs1-cbr.nexus.csiro.au\{ev-neap}\work\extent\processing\NEAP_intermediate\NVIS_PRE1750_IUCNGET_DK_20240809.tif</t>
   </si>
 </sst>
 </file>
@@ -566,7 +566,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -694,7 +694,7 @@
         <v>55</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>37</v>
@@ -729,7 +729,7 @@
         <v>56</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -761,7 +761,7 @@
         <v>48</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
@@ -831,7 +831,7 @@
         <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
@@ -866,7 +866,7 @@
         <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
         <v>36</v>
@@ -901,7 +901,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
         <v>36</v>

</xml_diff>